<commit_message>
Add check for of the pin details element exists
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -24,12 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
   <si>
     <t>KRA PIN</t>
   </si>
   <si>
     <t>A012263031Z</t>
+  </si>
+  <si>
+    <t>A012263031p</t>
+  </si>
+  <si>
+    <t>A012263039Z</t>
   </si>
 </sst>
 </file>
@@ -347,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A20"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -370,7 +376,7 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
@@ -390,72 +396,7 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>